<commit_message>
made notes on pre-sofltware dataset, need to revisit
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryAnalysis_Dataset_v6.xlsx
+++ b/DataRe-Analysis/SummaryAnalysis_Dataset_v6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="26920" windowHeight="15300" tabRatio="867"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="26920" windowHeight="15300" tabRatio="867" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies-PRE" sheetId="15" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7825" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7826" uniqueCount="1506">
   <si>
     <t>Organisms</t>
   </si>
@@ -4864,6 +4864,9 @@
   </si>
   <si>
     <t>Analysis for all resources: Predictive value</t>
+  </si>
+  <si>
+    <t>this is an algorithm, recheck</t>
   </si>
 </sst>
 </file>
@@ -5230,7 +5233,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5334,6 +5337,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -6193,7 +6202,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6856,6 +6865,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="732">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -8548,7 +8563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
@@ -33739,1625 +33754,1628 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="A63:XFD179"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="30"/>
-    <col min="2" max="2" width="17.33203125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="33.5" style="42" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="30"/>
-    <col min="7" max="7" width="15.83203125" style="30" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="30"/>
-    <col min="11" max="16384" width="10.83203125" style="30"/>
+    <col min="1" max="2" width="10.83203125" style="30"/>
+    <col min="3" max="3" width="17.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="33.5" style="42" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="30"/>
+    <col min="8" max="8" width="15.83203125" style="30" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="30"/>
+    <col min="12" max="16384" width="10.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="38" customFormat="1" ht="52">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:11" s="38" customFormat="1" ht="52">
+      <c r="B1" s="38" t="s">
         <v>983</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>1232</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="38" t="s">
         <v>1349</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>1350</v>
       </c>
-      <c r="F1" s="268" t="s">
+      <c r="G1" s="268" t="s">
         <v>1416</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>1233</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>1234</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="38" t="s">
         <v>976</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="270" customFormat="1" ht="39">
-      <c r="A2" s="269" t="s">
+    <row r="2" spans="1:11" s="270" customFormat="1" ht="39">
+      <c r="B2" s="269" t="s">
         <v>1401</v>
       </c>
-      <c r="C2" s="269"/>
-      <c r="F2" s="271" t="s">
+      <c r="D2" s="269"/>
+      <c r="G2" s="271" t="s">
         <v>1417</v>
       </c>
-      <c r="I2" s="270">
-        <f>COUNTIF(G4:G62,"y")</f>
+      <c r="J2" s="270">
+        <f>COUNTIF(H4:H62,"y")</f>
         <v>30</v>
       </c>
-      <c r="J2" s="270">
-        <f>COUNTA(C4:C62)</f>
+      <c r="K2" s="270">
+        <f>COUNTA(D4:D62)</f>
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="272" customFormat="1">
-      <c r="A3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="F3" s="273">
-        <f>COUNTIF(F4:F62,"NC")</f>
+    <row r="3" spans="1:11" s="272" customFormat="1">
+      <c r="B3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="G3" s="273">
+        <f>COUNTIF(G4:G62,"NC")</f>
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A4" s="274">
+    <row r="4" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B4" s="274">
         <v>23170245</v>
       </c>
-      <c r="B4" s="272" t="s">
+      <c r="C4" s="272" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="D4" s="141" t="s">
         <v>1235</v>
       </c>
-      <c r="D4" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G4" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A5" s="274">
+      <c r="H4" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" s="304" customFormat="1" ht="39">
+      <c r="B5" s="307">
         <v>23170245</v>
       </c>
-      <c r="B5" s="272" t="s">
+      <c r="C5" s="304" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="D5" s="305" t="s">
         <v>1236</v>
       </c>
-      <c r="D5" s="272" t="s">
+      <c r="E5" s="304" t="s">
         <v>414</v>
       </c>
-      <c r="E5" s="272" t="s">
+      <c r="F5" s="304" t="s">
         <v>414</v>
       </c>
-      <c r="F5" s="272" t="s">
+      <c r="G5" s="304" t="s">
         <v>1420</v>
       </c>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" s="272" customFormat="1">
-      <c r="A6" s="274">
+      <c r="K5" s="306"/>
+    </row>
+    <row r="6" spans="1:11" s="272" customFormat="1">
+      <c r="B6" s="274">
         <v>23170236</v>
       </c>
-      <c r="B6" s="272" t="s">
+      <c r="C6" s="272" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="D6" s="141" t="s">
         <v>1237</v>
       </c>
-      <c r="D6" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E6" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G6" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H6" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" s="272" customFormat="1">
-      <c r="A7" s="272">
+      <c r="I6" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B7" s="272">
         <v>24555100</v>
       </c>
-      <c r="B7" s="272" t="s">
+      <c r="C7" s="272" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="141" t="s">
+      <c r="D7" s="141" t="s">
         <v>1238</v>
       </c>
-      <c r="D7" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E7" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G7" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H7" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="272">
+      <c r="I7" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="272">
         <v>8</v>
       </c>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A8" s="272">
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B8" s="272">
         <v>22927320</v>
       </c>
-      <c r="B8" s="272" t="s">
+      <c r="C8" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="141" t="s">
+      <c r="D8" s="141" t="s">
         <v>1239</v>
       </c>
-      <c r="D8" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E8" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G8" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H8" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A9" s="272">
+        <v>3</v>
+      </c>
+      <c r="I8" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" s="272" customFormat="1">
+      <c r="B9" s="272">
         <v>22815064</v>
       </c>
-      <c r="B9" s="272" t="s">
+      <c r="C9" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="141" t="s">
+      <c r="D9" s="141" t="s">
         <v>1240</v>
       </c>
-      <c r="D9" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E9" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="272" t="s">
         <v>1407</v>
       </c>
-      <c r="F9" s="272" t="s">
+      <c r="G9" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G9" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" s="272" customFormat="1" ht="39">
-      <c r="A10" s="272">
+      <c r="H9" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B10" s="272">
         <v>22807169</v>
       </c>
-      <c r="B10" s="272" t="s">
+      <c r="C10" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="D10" s="141" t="s">
         <v>1241</v>
       </c>
-      <c r="D10" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E10" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G10" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H10" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" s="272" customFormat="1">
-      <c r="A11" s="272">
+      <c r="I10" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" s="304" customFormat="1">
+      <c r="A11" s="304" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B11" s="304">
         <v>22807169</v>
       </c>
-      <c r="B11" s="272" t="s">
+      <c r="C11" s="304" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="D11" s="305" t="s">
         <v>1242</v>
       </c>
-      <c r="D11" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="272" t="s">
+      <c r="E11" s="304" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="304" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="304" t="s">
         <v>1420</v>
       </c>
-      <c r="G11" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" s="272" customFormat="1">
-      <c r="A12" s="272">
+      <c r="H11" s="304" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="304" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="306"/>
+    </row>
+    <row r="12" spans="1:11" s="272" customFormat="1">
+      <c r="B12" s="272">
         <v>22807169</v>
       </c>
-      <c r="B12" s="272" t="s">
+      <c r="C12" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="141" t="s">
+      <c r="D12" s="141" t="s">
         <v>1243</v>
       </c>
-      <c r="D12" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E12" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F12" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G12" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H12" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A13" s="272">
+      <c r="I12" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B13" s="272">
         <v>22807169</v>
       </c>
-      <c r="B13" s="272" t="s">
+      <c r="C13" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="D13" s="141" t="s">
         <v>1244</v>
       </c>
-      <c r="D13" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E13" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G13" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H13" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" s="272" customFormat="1">
-      <c r="A14" s="272">
+        <v>3</v>
+      </c>
+      <c r="I13" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" s="272" customFormat="1" ht="39">
+      <c r="B14" s="272">
         <v>22807169</v>
       </c>
-      <c r="B14" s="272" t="s">
+      <c r="C14" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="141" t="s">
+      <c r="D14" s="141" t="s">
         <v>1245</v>
       </c>
-      <c r="D14" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E14" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F14" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G14" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H14" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A15" s="272">
+      <c r="I14" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" s="272" customFormat="1">
+      <c r="B15" s="272">
         <v>22777829</v>
       </c>
-      <c r="B15" s="272" t="s">
+      <c r="C15" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="D15" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G15" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H15" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" s="272" customFormat="1">
-      <c r="A16" s="272">
+        <v>7</v>
+      </c>
+      <c r="I15" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" s="272" customFormat="1" ht="26">
+      <c r="B16" s="272">
         <v>22707411</v>
       </c>
-      <c r="B16" s="272" t="s">
+      <c r="C16" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="141" t="s">
+      <c r="D16" s="141" t="s">
         <v>1246</v>
       </c>
-      <c r="D16" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E16" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G16" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H16" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" s="272" customFormat="1">
-      <c r="A17" s="272">
+        <v>3</v>
+      </c>
+      <c r="I16" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="2:11" s="272" customFormat="1">
+      <c r="B17" s="272">
         <v>22707411</v>
       </c>
-      <c r="B17" s="272" t="s">
+      <c r="C17" s="272" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="141" t="s">
+      <c r="D17" s="141" t="s">
         <v>1247</v>
       </c>
-      <c r="D17" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E17" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G17" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H17" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="1:10" s="272" customFormat="1">
-      <c r="A18" s="272">
+        <v>3</v>
+      </c>
+      <c r="I17" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="2:11" s="272" customFormat="1">
+      <c r="B18" s="272">
         <v>23065648</v>
       </c>
-      <c r="B18" s="272" t="s">
+      <c r="C18" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="141" t="s">
+      <c r="D18" s="141" t="s">
         <v>1248</v>
       </c>
-      <c r="D18" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E18" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G18" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H18" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="272">
+        <v>7</v>
+      </c>
+      <c r="I18" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="272">
         <v>8</v>
       </c>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" s="272" customFormat="1">
-      <c r="A19" s="272">
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="2:11" s="272" customFormat="1">
+      <c r="B19" s="272">
         <v>23065648</v>
       </c>
-      <c r="B19" s="272" t="s">
+      <c r="C19" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="141" t="s">
+      <c r="D19" s="141" t="s">
         <v>1249</v>
       </c>
-      <c r="D19" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E19" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G19" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H19" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="1:10" s="272" customFormat="1">
-      <c r="A20" s="272">
+      <c r="I19" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="2:11" s="272" customFormat="1">
+      <c r="B20" s="272">
         <v>23055045</v>
       </c>
-      <c r="B20" s="272" t="s">
+      <c r="C20" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="141" t="s">
+      <c r="D20" s="141" t="s">
         <v>1250</v>
       </c>
-      <c r="D20" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E20" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G20" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H20" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" s="272" customFormat="1">
-      <c r="A21" s="272">
+      <c r="I20" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="2:11" s="272" customFormat="1">
+      <c r="B21" s="272">
         <v>23055045</v>
       </c>
-      <c r="B21" s="272" t="s">
+      <c r="C21" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="141" t="s">
+      <c r="D21" s="141" t="s">
         <v>1251</v>
       </c>
-      <c r="D21" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E21" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G21" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H21" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A22" s="272">
+      <c r="I21" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="2:11" s="272" customFormat="1">
+      <c r="B22" s="272">
         <v>23055045</v>
       </c>
-      <c r="B22" s="272" t="s">
+      <c r="C22" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="141" t="s">
+      <c r="D22" s="141" t="s">
         <v>1249</v>
       </c>
-      <c r="D22" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E22" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F22" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G22" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H22" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" s="272" customFormat="1">
-      <c r="A23" s="272">
+      <c r="I22" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="2:11" s="272" customFormat="1">
+      <c r="B23" s="272">
         <v>23055045</v>
       </c>
-      <c r="B23" s="272" t="s">
+      <c r="C23" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="141" t="s">
+      <c r="D23" s="141" t="s">
         <v>1252</v>
       </c>
-      <c r="D23" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E23" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F23" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G23" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H23" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="1:10" s="272" customFormat="1" ht="52">
-      <c r="A24" s="272">
+        <v>7</v>
+      </c>
+      <c r="I23" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="2:11" s="272" customFormat="1">
+      <c r="B24" s="272">
         <v>23055045</v>
       </c>
-      <c r="B24" s="272" t="s">
+      <c r="C24" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="141" t="s">
+      <c r="D24" s="141" t="s">
         <v>1253</v>
       </c>
-      <c r="D24" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E24" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F24" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G24" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H24" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="1:10" s="272" customFormat="1">
-      <c r="A25" s="272">
+        <v>7</v>
+      </c>
+      <c r="I24" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="2:11" s="272" customFormat="1">
+      <c r="B25" s="272">
         <v>23055045</v>
       </c>
-      <c r="B25" s="272" t="s">
+      <c r="C25" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="141" t="s">
+      <c r="D25" s="141" t="s">
         <v>1254</v>
       </c>
-      <c r="D25" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E25" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F25" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G25" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H25" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A26" s="272">
+      <c r="I25" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B26" s="272">
         <v>23055043</v>
       </c>
-      <c r="B26" s="272" t="s">
+      <c r="C26" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="141" t="s">
+      <c r="D26" s="141" t="s">
         <v>1255</v>
       </c>
-      <c r="D26" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E26" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="272" t="s">
         <v>414</v>
       </c>
-      <c r="F26" s="272" t="s">
+      <c r="G26" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G26" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H26" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:10" s="272" customFormat="1">
-      <c r="A27" s="272">
+        <v>3</v>
+      </c>
+      <c r="I26" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B27" s="272">
         <v>22932976</v>
       </c>
-      <c r="B27" s="272" t="s">
+      <c r="C27" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="141" t="s">
+      <c r="D27" s="141" t="s">
         <v>1256</v>
       </c>
-      <c r="D27" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E27" s="272" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F27" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G27" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H27" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A28" s="272">
+      <c r="I27" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="2:11" s="272" customFormat="1">
+      <c r="B28" s="272">
         <v>22932976</v>
       </c>
-      <c r="B28" s="272" t="s">
+      <c r="C28" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="141" t="s">
+      <c r="D28" s="141" t="s">
         <v>1257</v>
       </c>
-      <c r="D28" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E28" s="272" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F28" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G28" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H28" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:10" s="272" customFormat="1">
-      <c r="A29" s="272">
+      <c r="I28" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="11"/>
+    </row>
+    <row r="29" spans="2:11" s="272" customFormat="1">
+      <c r="B29" s="272">
         <v>22932976</v>
       </c>
-      <c r="B29" s="272" t="s">
+      <c r="C29" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="141" t="s">
+      <c r="D29" s="141" t="s">
         <v>1258</v>
       </c>
-      <c r="D29" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E29" s="272" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F29" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G29" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H29" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A30" s="272">
+      <c r="I29" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B30" s="272">
         <v>22932976</v>
       </c>
-      <c r="B30" s="272" t="s">
+      <c r="C30" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="141" t="s">
+      <c r="D30" s="141" t="s">
         <v>1259</v>
       </c>
-      <c r="D30" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E30" s="272" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F30" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G30" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H30" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:10" s="272" customFormat="1">
-      <c r="A31" s="272">
+      <c r="I30" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="11"/>
+    </row>
+    <row r="31" spans="2:11" s="272" customFormat="1">
+      <c r="B31" s="272">
         <v>22903439</v>
       </c>
-      <c r="B31" s="272" t="s">
+      <c r="C31" s="272" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="141" t="s">
+      <c r="D31" s="141" t="s">
         <v>1260</v>
       </c>
-      <c r="D31" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E31" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G31" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H31" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="1:10" s="272" customFormat="1">
-      <c r="A32" s="272">
+      <c r="I31" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="11"/>
+    </row>
+    <row r="32" spans="2:11" s="272" customFormat="1">
+      <c r="B32" s="272">
         <v>23184649</v>
       </c>
-      <c r="B32" s="272" t="s">
+      <c r="C32" s="272" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="141" t="s">
+      <c r="D32" s="141" t="s">
         <v>1261</v>
       </c>
-      <c r="D32" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E32" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G32" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H32" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="11"/>
-    </row>
-    <row r="33" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A33" s="272">
+        <v>3</v>
+      </c>
+      <c r="I32" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B33" s="272">
         <v>22407500</v>
       </c>
-      <c r="B33" s="272" t="s">
+      <c r="C33" s="272" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="141" t="s">
+      <c r="D33" s="141" t="s">
         <v>1262</v>
       </c>
-      <c r="D33" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E33" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F33" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G33" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H33" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J33" s="11"/>
-    </row>
-    <row r="34" spans="1:10" s="272" customFormat="1" ht="39">
-      <c r="A34" s="272">
+        <v>3</v>
+      </c>
+      <c r="I33" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="11"/>
+    </row>
+    <row r="34" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B34" s="272">
         <v>22144346</v>
       </c>
-      <c r="B34" s="272" t="s">
+      <c r="C34" s="272" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="141" t="s">
+      <c r="D34" s="141" t="s">
         <v>1263</v>
       </c>
-      <c r="D34" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E34" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G34" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H34" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J34" s="11"/>
-    </row>
-    <row r="35" spans="1:10" s="272" customFormat="1">
-      <c r="A35" s="272">
+        <v>3</v>
+      </c>
+      <c r="I34" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B35" s="272">
         <v>21830163</v>
       </c>
-      <c r="B35" s="272" t="s">
+      <c r="C35" s="272" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="141" t="s">
+      <c r="D35" s="141" t="s">
         <v>1264</v>
       </c>
-      <c r="D35" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E35" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F35" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G35" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H35" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="11"/>
-    </row>
-    <row r="36" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A36" s="272">
+        <v>3</v>
+      </c>
+      <c r="I35" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" spans="2:11" s="272" customFormat="1">
+      <c r="B36" s="272">
         <v>23638346</v>
       </c>
-      <c r="B36" s="272" t="s">
+      <c r="C36" s="272" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="141" t="s">
+      <c r="D36" s="141" t="s">
         <v>1265</v>
       </c>
-      <c r="D36" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E36" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F36" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G36" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" s="272">
+      <c r="H36" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="272">
         <v>9</v>
       </c>
-      <c r="J36" s="11"/>
-    </row>
-    <row r="37" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A37" s="272">
+      <c r="K36" s="11"/>
+    </row>
+    <row r="37" spans="2:11" s="272" customFormat="1">
+      <c r="B37" s="272">
         <v>23638349</v>
       </c>
-      <c r="B37" s="272" t="s">
+      <c r="C37" s="272" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="141" t="s">
+      <c r="D37" s="141" t="s">
         <v>1266</v>
       </c>
-      <c r="D37" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E37" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F37" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G37" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H37" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="1:10" s="272" customFormat="1">
-      <c r="A38" s="272">
+        <v>7</v>
+      </c>
+      <c r="I37" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="11"/>
+    </row>
+    <row r="38" spans="2:11" s="272" customFormat="1">
+      <c r="B38" s="272">
         <v>23638367</v>
       </c>
-      <c r="B38" s="272" t="s">
+      <c r="C38" s="272" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="141" t="s">
+      <c r="D38" s="141" t="s">
         <v>1267</v>
       </c>
-      <c r="D38" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E38" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F38" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G38" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H38" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39" spans="1:10" s="272" customFormat="1">
-      <c r="A39" s="272">
+      <c r="I38" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="11"/>
+    </row>
+    <row r="39" spans="2:11" s="272" customFormat="1">
+      <c r="B39" s="272">
         <v>23420185</v>
       </c>
-      <c r="B39" s="272" t="s">
+      <c r="C39" s="272" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="141" t="s">
+      <c r="D39" s="141" t="s">
         <v>1268</v>
       </c>
-      <c r="D39" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E39" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G39" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H39" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J39" s="11"/>
-    </row>
-    <row r="40" spans="1:10" s="272" customFormat="1">
-      <c r="A40" s="272">
+      <c r="I39" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" s="11"/>
+    </row>
+    <row r="40" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B40" s="272">
         <v>23508232</v>
       </c>
-      <c r="B40" s="272" t="s">
+      <c r="C40" s="272" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="141" t="s">
+      <c r="D40" s="141" t="s">
         <v>1269</v>
       </c>
-      <c r="D40" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E40" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G40" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H40" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J40" s="11"/>
-    </row>
-    <row r="41" spans="1:10" s="272" customFormat="1">
-      <c r="A41" s="272">
+      <c r="I40" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="11"/>
+    </row>
+    <row r="41" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B41" s="272">
         <v>23717278</v>
       </c>
-      <c r="B41" s="272" t="s">
+      <c r="C41" s="272" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="141" t="s">
+      <c r="D41" s="141" t="s">
         <v>1270</v>
       </c>
-      <c r="D41" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E41" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F41" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G41" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H41" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J41" s="11"/>
-    </row>
-    <row r="42" spans="1:10" s="272" customFormat="1">
-      <c r="A42" s="272">
+      <c r="I41" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="11"/>
+    </row>
+    <row r="42" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B42" s="272">
         <v>23717278</v>
       </c>
-      <c r="B42" s="272" t="s">
+      <c r="C42" s="272" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="141" t="s">
+      <c r="D42" s="141" t="s">
         <v>1271</v>
       </c>
-      <c r="D42" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E42" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F42" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G42" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="H42" s="272" t="s">
         <v>3</v>
       </c>
-      <c r="J42" s="11"/>
-    </row>
-    <row r="43" spans="1:10" s="272" customFormat="1">
-      <c r="A43" s="272">
+      <c r="I42" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="11"/>
+    </row>
+    <row r="43" spans="2:11" s="272" customFormat="1">
+      <c r="B43" s="272">
         <v>23322532</v>
       </c>
-      <c r="B43" s="272" t="s">
+      <c r="C43" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C43" s="141" t="s">
+      <c r="D43" s="141" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E43" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G43" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="1:10" s="272" customFormat="1">
-      <c r="A44" s="272">
+      <c r="H43" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="11"/>
+    </row>
+    <row r="44" spans="2:11" s="272" customFormat="1" ht="39">
+      <c r="B44" s="272">
         <v>23322547</v>
       </c>
-      <c r="B44" s="272" t="s">
+      <c r="C44" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C44" s="141" t="s">
+      <c r="D44" s="141" t="s">
         <v>1273</v>
       </c>
-      <c r="D44" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E44" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F44" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G44" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J44" s="11"/>
-    </row>
-    <row r="45" spans="1:10" s="272" customFormat="1">
-      <c r="A45" s="272">
+      <c r="H44" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K44" s="11"/>
+    </row>
+    <row r="45" spans="2:11" s="272" customFormat="1">
+      <c r="B45" s="272">
         <v>22736487</v>
       </c>
-      <c r="B45" s="272" t="s">
+      <c r="C45" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C45" s="141" t="s">
+      <c r="D45" s="141" t="s">
         <v>1274</v>
       </c>
-      <c r="D45" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E45" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F45" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G45" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="1:10" s="272" customFormat="1">
-      <c r="A46" s="272">
+      <c r="H45" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="11"/>
+    </row>
+    <row r="46" spans="2:11" s="272" customFormat="1">
+      <c r="B46" s="272">
         <v>10777769</v>
       </c>
-      <c r="B46" s="272" t="s">
+      <c r="C46" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C46" s="275" t="s">
+      <c r="D46" s="275" t="s">
         <v>1275</v>
       </c>
-      <c r="D46" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E46" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F46" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G46" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" s="272" customFormat="1">
-      <c r="A47" s="272">
+      <c r="H46" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="2:11" s="272" customFormat="1">
+      <c r="B47" s="272">
         <v>11027223</v>
       </c>
-      <c r="B47" s="272" t="s">
+      <c r="C47" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C47" s="275" t="s">
+      <c r="D47" s="275" t="s">
         <v>1275</v>
       </c>
-      <c r="D47" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E47" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F47" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G47" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J47" s="11"/>
-    </row>
-    <row r="48" spans="1:10" s="272" customFormat="1">
-      <c r="A48" s="272">
+      <c r="H47" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="11"/>
+    </row>
+    <row r="48" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B48" s="272">
         <v>15901783</v>
       </c>
-      <c r="B48" s="272" t="s">
+      <c r="C48" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C48" s="275" t="s">
+      <c r="D48" s="275" t="s">
         <v>1276</v>
       </c>
-      <c r="D48" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E48" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F48" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G48" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H48" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J48" s="11"/>
-    </row>
-    <row r="49" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A49" s="272">
+        <v>7</v>
+      </c>
+      <c r="I48" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K48" s="11"/>
+    </row>
+    <row r="49" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B49" s="272">
         <v>17522311</v>
       </c>
-      <c r="B49" s="272" t="s">
+      <c r="C49" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C49" s="275" t="s">
+      <c r="D49" s="275" t="s">
         <v>1277</v>
       </c>
-      <c r="D49" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E49" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F49" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G49" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J49" s="11"/>
-    </row>
-    <row r="50" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A50" s="272">
+      <c r="H49" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K49" s="11"/>
+    </row>
+    <row r="50" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B50" s="272">
         <v>19474329</v>
       </c>
-      <c r="B50" s="272" t="s">
+      <c r="C50" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C50" s="275" t="s">
+      <c r="D50" s="275" t="s">
         <v>1278</v>
       </c>
-      <c r="D50" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E50" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F50" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G50" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J50" s="11"/>
-    </row>
-    <row r="51" spans="1:10" s="272" customFormat="1">
-      <c r="A51" s="272">
+      <c r="H50" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K50" s="11"/>
+    </row>
+    <row r="51" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B51" s="272">
         <v>22553016</v>
       </c>
-      <c r="B51" s="272" t="s">
+      <c r="C51" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C51" s="275" t="s">
+      <c r="D51" s="275" t="s">
         <v>1279</v>
       </c>
-      <c r="D51" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E51" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F51" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G51" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J51" s="11"/>
-    </row>
-    <row r="52" spans="1:10" s="272" customFormat="1">
-      <c r="A52" s="272">
+      <c r="H51" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="2:11" s="272" customFormat="1">
+      <c r="B52" s="272">
         <v>23365253</v>
       </c>
-      <c r="B52" s="272" t="s">
+      <c r="C52" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C52" s="275" t="s">
+      <c r="D52" s="275" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E52" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F52" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G52" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="11"/>
-    </row>
-    <row r="53" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A53" s="272">
+      <c r="H52" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52" s="11"/>
+    </row>
+    <row r="53" spans="2:11" s="272" customFormat="1">
+      <c r="B53" s="272">
         <v>17093092</v>
       </c>
-      <c r="B53" s="272" t="s">
+      <c r="C53" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C53" s="275" t="s">
+      <c r="D53" s="275" t="s">
         <v>1280</v>
       </c>
-      <c r="D53" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E53" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F53" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G53" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="11"/>
-    </row>
-    <row r="54" spans="1:10" s="272" customFormat="1">
-      <c r="A54" s="272">
+      <c r="H53" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53" s="11"/>
+    </row>
+    <row r="54" spans="2:11" s="272" customFormat="1">
+      <c r="B54" s="272">
         <v>22674266</v>
       </c>
-      <c r="B54" s="272" t="s">
+      <c r="C54" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C54" s="275" t="s">
+      <c r="D54" s="275" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E54" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F54" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G54" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="11"/>
-    </row>
-    <row r="55" spans="1:10" s="272" customFormat="1" ht="39">
-      <c r="A55" s="272">
+      <c r="H54" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K54" s="11"/>
+    </row>
+    <row r="55" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B55" s="272">
         <v>23325254</v>
       </c>
-      <c r="B55" s="272" t="s">
+      <c r="C55" s="272" t="s">
         <v>1272</v>
       </c>
-      <c r="C55" s="275" t="s">
+      <c r="D55" s="275" t="s">
         <v>1281</v>
       </c>
-      <c r="D55" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E55" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F55" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G55" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J55" s="11"/>
-    </row>
-    <row r="56" spans="1:10" s="272" customFormat="1">
-      <c r="A56" s="272">
+      <c r="H55" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K55" s="11"/>
+    </row>
+    <row r="56" spans="2:11" s="272" customFormat="1">
+      <c r="B56" s="272">
         <v>23106570</v>
       </c>
-      <c r="B56" s="272" t="s">
+      <c r="C56" s="272" t="s">
         <v>1071</v>
       </c>
-      <c r="C56" s="141" t="s">
+      <c r="D56" s="141" t="s">
         <v>1282</v>
       </c>
-      <c r="D56" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E56" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F56" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G56" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="I56" s="272">
+      <c r="H56" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="272">
         <v>4</v>
       </c>
-      <c r="J56" s="11"/>
-    </row>
-    <row r="57" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A57" s="272">
+      <c r="K56" s="11"/>
+    </row>
+    <row r="57" spans="2:11" s="272" customFormat="1" ht="26">
+      <c r="B57" s="272">
         <v>23106436</v>
       </c>
-      <c r="B57" s="272" t="s">
+      <c r="C57" s="272" t="s">
         <v>1071</v>
       </c>
-      <c r="C57" s="141" t="s">
+      <c r="D57" s="141" t="s">
         <v>1283</v>
       </c>
-      <c r="D57" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E57" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F57" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G57" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J57" s="11"/>
-    </row>
-    <row r="58" spans="1:10" s="272" customFormat="1">
-      <c r="A58" s="272">
+      <c r="H57" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K57" s="11"/>
+    </row>
+    <row r="58" spans="2:11" s="272" customFormat="1">
+      <c r="B58" s="272">
         <v>23106536</v>
       </c>
-      <c r="B58" s="272" t="s">
+      <c r="C58" s="272" t="s">
         <v>1071</v>
       </c>
-      <c r="C58" s="141" t="s">
+      <c r="D58" s="141" t="s">
         <v>1284</v>
       </c>
-      <c r="D58" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="E58" s="272" t="s">
         <v>7</v>
       </c>
       <c r="F58" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G58" s="272" t="s">
-        <v>7</v>
-      </c>
       <c r="H58" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="J58" s="11"/>
-    </row>
-    <row r="59" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A59" s="272">
+      <c r="I58" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K58" s="11"/>
+    </row>
+    <row r="59" spans="2:11" s="272" customFormat="1">
+      <c r="B59" s="272">
         <v>22269797</v>
       </c>
-      <c r="B59" s="272" t="s">
+      <c r="C59" s="272" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="141" t="s">
+      <c r="D59" s="141" t="s">
         <v>1285</v>
       </c>
-      <c r="D59" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E59" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F59" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G59" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J59" s="11"/>
-    </row>
-    <row r="60" spans="1:10" s="272" customFormat="1">
-      <c r="A60" s="272">
+      <c r="H59" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="11"/>
+    </row>
+    <row r="60" spans="2:11" s="272" customFormat="1">
+      <c r="B60" s="272">
         <v>23295855</v>
       </c>
-      <c r="B60" s="272" t="s">
+      <c r="C60" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="276" t="s">
+      <c r="D60" s="276" t="s">
         <v>1286</v>
       </c>
-      <c r="D60" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E60" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F60" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G60" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="I60" s="272">
-        <v>3</v>
-      </c>
-      <c r="J60" s="11"/>
-    </row>
-    <row r="61" spans="1:10" s="272" customFormat="1">
-      <c r="A61" s="272">
+      <c r="H60" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="J60" s="272">
+        <v>3</v>
+      </c>
+      <c r="K60" s="11"/>
+    </row>
+    <row r="61" spans="2:11" s="272" customFormat="1">
+      <c r="B61" s="272">
         <v>23295857</v>
       </c>
-      <c r="B61" s="272" t="s">
+      <c r="C61" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="276" t="s">
+      <c r="D61" s="276" t="s">
         <v>1287</v>
       </c>
-      <c r="D61" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E61" s="272" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F61" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G61" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="J61" s="11"/>
-    </row>
-    <row r="62" spans="1:10" s="272" customFormat="1" ht="26">
-      <c r="A62" s="272">
+      <c r="H61" s="272" t="s">
+        <v>7</v>
+      </c>
+      <c r="K61" s="11"/>
+    </row>
+    <row r="62" spans="2:11" s="272" customFormat="1">
+      <c r="B62" s="272">
         <v>23313314</v>
       </c>
-      <c r="B62" s="272" t="s">
+      <c r="C62" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="141" t="s">
+      <c r="D62" s="141" t="s">
         <v>1288</v>
       </c>
-      <c r="D62" s="272" t="s">
-        <v>3</v>
-      </c>
       <c r="E62" s="272" t="s">
         <v>3</v>
       </c>
       <c r="F62" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="272" t="s">
         <v>1420</v>
       </c>
-      <c r="G62" s="272" t="s">
-        <v>3</v>
-      </c>
-      <c r="J62" s="11"/>
+      <c r="H62" s="272" t="s">
+        <v>3</v>
+      </c>
+      <c r="K62" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A4:J179">
-    <sortCondition descending="1" ref="F4:F179"/>
+  <sortState ref="B4:K179">
+    <sortCondition descending="1" ref="G4:G179"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -42074,11 +42092,11 @@
         <v>0.50847457627118642</v>
       </c>
       <c r="C13" s="107">
+        <f>'Software-PRE'!K2</f>
+        <v>59</v>
+      </c>
+      <c r="D13" s="110">
         <f>'Software-PRE'!J2</f>
-        <v>59</v>
-      </c>
-      <c r="D13" s="110">
-        <f>'Software-PRE'!I2</f>
         <v>30</v>
       </c>
     </row>

</xml_diff>